<commit_message>
Plotted the the number of students by career paths chosen
</commit_message>
<xml_diff>
--- a/assets/GeneralAssembly.xlsx
+++ b/assets/GeneralAssembly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://metrouw-my.sharepoint.com/personal/gwen_duncan_metrounitedway_org/Documents/Desktop/Professional Development/Python/Code_Louisville/data_1_checks/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{94DE0868-5322-4A62-9E04-C335A2C37D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FFD4963-1050-481A-BC04-2BF94D009486}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{94DE0868-5322-4A62-9E04-C335A2C37D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB2916B8-FC61-46D5-AB37-4EC33D928BFD}"/>
   <bookViews>
-    <workbookView xWindow="-156" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SurveyMonkey" sheetId="5" r:id="rId1"/>
@@ -2120,7 +2120,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B61074D8-FACD-49C2-B129-BCDA1CC60808}" name="Table13" displayName="Table13" ref="A1:Z104" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:Z104" xr:uid="{87A9D076-61F9-4164-914B-6050329614B3}"/>
+  <autoFilter ref="A1:Z104" xr:uid="{87A9D076-61F9-4164-914B-6050329614B3}">
+    <filterColumn colId="20">
+      <filters>
+        <filter val="Data analytics"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{5751402A-A723-4B64-94C5-DA8B44FFE57D}" name="Respondent ID" dataDxfId="25"/>
     <tableColumn id="2" xr3:uid="{AAE68CA8-140F-4459-9BA6-E3A988AE3869}" name="Collector ID" dataDxfId="24"/>
@@ -2357,7 +2363,7 @@
   <dimension ref="A1:Z104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="U1" sqref="U1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2536,7 +2542,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>12280807493</v>
       </c>
@@ -2612,7 +2618,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>12000201515</v>
       </c>
@@ -2841,7 +2847,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>12309689608</v>
       </c>
@@ -3141,7 +3147,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>12059654513</v>
       </c>
@@ -3219,7 +3225,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>12002504867</v>
       </c>
@@ -3297,7 +3303,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>12290701753</v>
       </c>
@@ -3375,7 +3381,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>12275610241</v>
       </c>
@@ -3527,7 +3533,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>12298025821</v>
       </c>
@@ -3607,7 +3613,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>12016192116</v>
       </c>
@@ -3841,7 +3847,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>12373053779</v>
       </c>
@@ -4219,7 +4225,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>12002528221</v>
       </c>
@@ -4447,7 +4453,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>12097152815</v>
       </c>
@@ -4607,7 +4613,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>12069990694</v>
       </c>
@@ -4838,7 +4844,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
         <v>12303682123</v>
       </c>
@@ -5300,7 +5306,7 @@
       </c>
       <c r="Z38" s="19"/>
     </row>
-    <row r="39" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
         <v>12257749162</v>
       </c>
@@ -5378,7 +5384,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11">
         <v>12060109727</v>
       </c>
@@ -6075,7 +6081,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11">
         <v>12270085164</v>
       </c>
@@ -6150,7 +6156,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11">
         <v>12503401190</v>
       </c>
@@ -6224,7 +6230,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11">
         <v>12314918073</v>
       </c>
@@ -6375,7 +6381,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11">
         <v>12288576221</v>
       </c>
@@ -6530,7 +6536,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11">
         <v>12007848693</v>
       </c>
@@ -6607,7 +6613,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <v>12082760922</v>
       </c>
@@ -6682,7 +6688,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11">
         <v>12270231147</v>
       </c>
@@ -6758,7 +6764,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11">
         <v>12004758637</v>
       </c>
@@ -6915,7 +6921,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11">
         <v>12270133363</v>
       </c>
@@ -7068,7 +7074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11">
         <v>12086462967</v>
       </c>
@@ -7296,7 +7302,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>12462700309</v>
       </c>
@@ -7374,7 +7380,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
         <v>12762452908</v>
       </c>
@@ -7524,7 +7530,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
         <v>12003647859</v>
       </c>
@@ -7756,7 +7762,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="11">
         <v>12028349522</v>
       </c>
@@ -7987,7 +7993,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="11">
         <v>12045999848</v>
       </c>
@@ -8145,7 +8151,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="11">
         <v>12013437566</v>
       </c>
@@ -8221,7 +8227,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11">
         <v>12014799080</v>
       </c>
@@ -8296,7 +8302,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="11">
         <v>12000285183</v>
       </c>
@@ -8758,7 +8764,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="11">
         <v>12001489408</v>
       </c>
@@ -8834,7 +8840,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="85" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="11">
         <v>12217273795</v>
       </c>
@@ -8909,7 +8915,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="11">
         <v>12419880645</v>
       </c>
@@ -9066,7 +9072,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="11">
         <v>12273135425</v>
       </c>
@@ -9367,7 +9373,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="11">
         <v>12026837182</v>
       </c>
@@ -9444,7 +9450,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="11">
         <v>12097591041</v>
       </c>
@@ -9675,7 +9681,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="11">
         <v>12056408926</v>
       </c>
@@ -9753,7 +9759,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="11">
         <v>12042991972</v>
       </c>
@@ -9830,7 +9836,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="11">
         <v>12270120670</v>
       </c>
@@ -10139,7 +10145,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="11">
         <v>12087727949</v>
       </c>
@@ -10214,7 +10220,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="11">
         <v>12535044829</v>
       </c>

</xml_diff>

<commit_message>
Changed plot to pull from excel file instead of list
</commit_message>
<xml_diff>
--- a/assets/GeneralAssembly.xlsx
+++ b/assets/GeneralAssembly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://metrouw-my.sharepoint.com/personal/gwen_duncan_metrounitedway_org/Documents/Desktop/Professional Development/Python/Code_Louisville/data_1_checks/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{94DE0868-5322-4A62-9E04-C335A2C37D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB2916B8-FC61-46D5-AB37-4EC33D928BFD}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="8_{94DE0868-5322-4A62-9E04-C335A2C37D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D04ACFCA-FEE6-4A05-A747-B122FB7330BE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2382,7 +2382,9 @@
     <col min="16" max="16" width="57.109375" customWidth="1"/>
     <col min="18" max="18" width="57.109375" customWidth="1"/>
     <col min="19" max="19" width="56" customWidth="1"/>
-    <col min="20" max="23" width="57.109375" customWidth="1"/>
+    <col min="20" max="20" width="57.109375" customWidth="1"/>
+    <col min="21" max="21" width="62" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="57.109375" customWidth="1"/>
     <col min="24" max="25" width="48.33203125" customWidth="1"/>
     <col min="26" max="26" width="45.109375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>